<commit_message>
Visualized plots comparing subscales of SF-36 to US Gen Pop
</commit_message>
<xml_diff>
--- a/!SF36_CompositeScores.xlsx
+++ b/!SF36_CompositeScores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Scale</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>stdErr</t>
   </si>
   <si>
     <t>stdDev</t>
@@ -201,38 +204,47 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
         <v>46.6</v>
       </c>
       <c r="E2" t="n">
+        <v>1.6439817267480255</v>
+      </c>
+      <c r="F2" t="n">
         <v>3.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
         <v>45.5</v>
       </c>
       <c r="E3" t="n">
+        <v>1.6884466964922387</v>
+      </c>
+      <c r="F3" t="n">
         <v>3.8</v>
       </c>
     </row>
@@ -258,7 +270,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -266,16 +278,19 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="n">
         <v>0.47619047619047616</v>
@@ -284,18 +299,21 @@
         <v>-0.5</v>
       </c>
       <c r="F2" t="n">
+        <v>0.2537454844043347</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" t="n">
         <v>0.19047619047619047</v>
@@ -304,18 +322,21 @@
         <v>-1.0</v>
       </c>
       <c r="F3" t="n">
+        <v>0.8665906719226351</v>
+      </c>
+      <c r="G3" t="n">
         <v>1.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
         <v>0.09523809523809523</v>
@@ -324,18 +345,21 @@
         <v>0.3</v>
       </c>
       <c r="F4" t="n">
+        <v>0.5733462746497072</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="n">
         <v>0.23809523809523808</v>
@@ -344,18 +368,21 @@
         <v>0.2</v>
       </c>
       <c r="F5" t="n">
+        <v>0.5099185101981403</v>
+      </c>
+      <c r="G5" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
         <v>0.2857142857142857</v>
@@ -364,18 +391,21 @@
         <v>-0.2</v>
       </c>
       <c r="F6" t="n">
+        <v>0.6299374464434435</v>
+      </c>
+      <c r="G6" t="n">
         <v>1.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="n">
         <v>0.14285714285714285</v>
@@ -384,18 +414,21 @@
         <v>-0.3</v>
       </c>
       <c r="F7" t="n">
+        <v>0.43960691722598305</v>
+      </c>
+      <c r="G7" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
         <v>0.21428571428571427</v>
@@ -404,18 +437,21 @@
         <v>-0.9</v>
       </c>
       <c r="F8" t="n">
+        <v>0.5081300813008129</v>
+      </c>
+      <c r="G8" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="n">
         <v>0.35714285714285715</v>
@@ -424,6 +460,9 @@
         <v>-0.5</v>
       </c>
       <c r="F9" t="n">
+        <v>0.4666244995430623</v>
+      </c>
+      <c r="G9" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -449,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -457,16 +496,19 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="n">
         <v>0.47619047619047616</v>
@@ -475,18 +517,21 @@
         <v>44.0</v>
       </c>
       <c r="F2" t="n">
+        <v>3.674234614174767</v>
+      </c>
+      <c r="G2" t="n">
         <v>8.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" t="n">
         <v>0.19047619047619047</v>
@@ -495,18 +540,21 @@
         <v>35.0</v>
       </c>
       <c r="F3" t="n">
+        <v>12.74754878398196</v>
+      </c>
+      <c r="G3" t="n">
         <v>28.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
         <v>0.09523809523809523</v>
@@ -515,18 +563,21 @@
         <v>55.5</v>
       </c>
       <c r="F4" t="n">
+        <v>9.334077351297235</v>
+      </c>
+      <c r="G4" t="n">
         <v>20.9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
         <v>0.23809523809523808</v>
@@ -535,18 +586,21 @@
         <v>53.0</v>
       </c>
       <c r="F5" t="n">
+        <v>8.602325267042625</v>
+      </c>
+      <c r="G5" t="n">
         <v>19.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="n">
         <v>0.2857142857142857</v>
@@ -555,18 +609,21 @@
         <v>51.0</v>
       </c>
       <c r="F6" t="n">
+        <v>9.669539802906858</v>
+      </c>
+      <c r="G6" t="n">
         <v>21.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="n">
         <v>0.14285714285714285</v>
@@ -575,18 +632,21 @@
         <v>47.5</v>
       </c>
       <c r="F7" t="n">
+        <v>6.123724356957945</v>
+      </c>
+      <c r="G7" t="n">
         <v>13.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="n">
         <v>0.21428571428571427</v>
@@ -595,18 +655,21 @@
         <v>40.0</v>
       </c>
       <c r="F8" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="G8" t="n">
         <v>14.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="n">
         <v>0.35714285714285715</v>
@@ -615,6 +678,9 @@
         <v>48.0</v>
       </c>
       <c r="F9" t="n">
+        <v>6.196773353931866</v>
+      </c>
+      <c r="G9" t="n">
         <v>13.9</v>
       </c>
     </row>

</xml_diff>